<commit_message>
updated query in gender script ctdc
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A5A05C-CC2A-4FAE-A016-8FFEA0CFC86A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5CAFDB-DDEE-4A8E-8DBB-3FFCF744EFD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -48,13 +48,36 @@
     <t>TC01_Trials_Filter_Gender-Male_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.gender IN ['MALE'] RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(t.clinical_trial_designation ,'')as `Trial Code` , coalesce(a.arm_id,'') As `Arm` , coalesce(a.arm_drug,'') As `Arm Treatment` , coalesce(c.disease,'') As Diagnosis , coalesce(c.gender,'') As Gender , coalesce(c.race,'') As Race , coalesce(c.ethnicity,'') As Ethnicity</t>
-  </si>
-  <si>
     <t>StatQuery</t>
   </si>
   <si>
-    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.gender IN ['MALE']  OPTIONAL MATCH (s)&lt;-[*]-(f:file) RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(t.clinical_trial_designation)) as number_of_trial</t>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ct:clinical_trial)&lt;--(a:arm)&lt;--(c:case)
+    WHERE c.gender = "MALE"
+WITH DISTINCT c, a, ct
+RETURN 
+    COALESCE(c.case_id, '') AS `Case ID`,
+    COALESCE(ct.clinical_trial_designation, '') AS `Trial Code`,
+    COALESCE(a.arm_id, '') AS `Arm`,
+    COALESCE(a.arm_drug, '') AS `Arm Treatment`,
+    COALESCE(c.disease, '') AS `Diagnosis`,
+    COALESCE(c.gender, '') AS `Gender`,
+    COALESCE(c.race, '') AS `Race`,
+    COALESCE(c.ethnicity, '') AS `Ethnicity`</t>
+  </si>
+  <si>
+    <t>MATCH (s:specimen)--&gt;(c:case)--&gt;(:arm)--&gt;(ct:clinical_trial)
+    WHERE c.gender = "MALE"
+OPTIONAL MATCH (f:file)--&gt;(:sequencing_assay)--&gt;(:nucleic_acid)--&gt;(s)
+RETURN 
+    COUNT(DISTINCT f) AS number_of_files,
+    COUNT(DISTINCT c.case_id) AS number_of_cases,
+    COUNT(DISTINCT ct.clinical_trial_designation) AS number_of_trials</t>
   </si>
 </sst>
 </file>
@@ -424,44 +447,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
+    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated gender xls with filetab query
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5CAFDB-DDEE-4A8E-8DBB-3FFCF744EFD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7619E4-12F3-474F-A7D6-6DEB945EB8B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>WebExcel</t>
   </si>
@@ -78,6 +78,24 @@
     COUNT(DISTINCT f) AS number_of_files,
     COUNT(DISTINCT c.case_id) AS number_of_cases,
     COUNT(DISTINCT ct.clinical_trial_designation) AS number_of_trials</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ct:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;-[*]-(prt)&lt;--(f:file)
+    WHERE c.gender = "MALE"
+WITH DISTINCT f, prt, c, a, ct
+RETURN
+    COALESCE(f.file_name, '') AS `File Name`,
+    COALESCE(head(labels(prt)), '') AS `Association`,
+​
+    COALESCE(f.file_description, '') AS `Description`,
+    COALESCE(f.file_format, '') AS `File Format`,
+    COALESCE(f.file_size, '') AS `Size`,
+    COALESCE(ct.clinical_trial_designation, '') AS `Trial Code`,
+    COALESCE(a.arm_id, '') AS `Arm`,
+    COALESCE(c.case_id, '') AS `Case ID`</t>
   </si>
 </sst>
 </file>
@@ -447,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,6 +513,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added objects in stage of disease icdc
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7619E4-12F3-474F-A7D6-6DEB945EB8B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D356F9-3AE1-4CDC-9E10-C8B0D58BBE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -57,45 +57,64 @@
     <t>CasesTab</t>
   </si>
   <si>
-    <t>MATCH (ct:clinical_trial)&lt;--(a:arm)&lt;--(c:case)
-    WHERE c.gender = "MALE"
-WITH DISTINCT c, a, ct
-RETURN 
-    COALESCE(c.case_id, '') AS `Case ID`,
-    COALESCE(ct.clinical_trial_designation, '') AS `Trial Code`,
-    COALESCE(a.arm_id, '') AS `Arm`,
-    COALESCE(a.arm_drug, '') AS `Arm Treatment`,
-    COALESCE(c.disease, '') AS `Diagnosis`,
-    COALESCE(c.gender, '') AS `Gender`,
-    COALESCE(c.race, '') AS `Race`,
-    COALESCE(c.ethnicity, '') AS `Ethnicity`</t>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (c:case)
+    WHERE c.gender='MALE'
+OPTIONAL MATCH (c)-[:of_arm]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+RETURN DISTINCT
+    c.case_id AS `Case ID`,
+     ct.clinical_trial_designation AS `Trial Code`,
+     a.arm_id AS Arm,
+      a.arm_drug AS `Arm Treatment`,
+c.disease AS Diagnosis,
+  c.gender AS Gender,
+    c.race AS Race,
+    c.ethnicity AS Ethnicity
+ </t>
   </si>
   <si>
     <t>MATCH (s:specimen)--&gt;(c:case)--&gt;(:arm)--&gt;(ct:clinical_trial)
     WHERE c.gender = "MALE"
 OPTIONAL MATCH (f:file)--&gt;(:sequencing_assay)--&gt;(:nucleic_acid)--&gt;(s)
 RETURN 
-    COUNT(DISTINCT f) AS number_of_files,
-    COUNT(DISTINCT c.case_id) AS number_of_cases,
-    COUNT(DISTINCT ct.clinical_trial_designation) AS number_of_trials</t>
-  </si>
-  <si>
-    <t>FilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (ct:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;-[*]-(prt)&lt;--(f:file)
-    WHERE c.gender = "MALE"
-WITH DISTINCT f, prt, c, a, ct
-RETURN
-    COALESCE(f.file_name, '') AS `File Name`,
-    COALESCE(head(labels(prt)), '') AS `Association`,
-​
-    COALESCE(f.file_description, '') AS `Description`,
-    COALESCE(f.file_format, '') AS `File Format`,
-    COALESCE(f.file_size, '') AS `Size`,
-    COALESCE(ct.clinical_trial_designation, '') AS `Trial Code`,
-    COALESCE(a.arm_id, '') AS `Arm`,
-    COALESCE(c.case_id, '') AS `Case ID`</t>
+     COUNT(DISTINCT ct.clinical_trial_designation) AS Trials,
+     COUNT(DISTINCT c.case_id) AS Cases,
+      COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MATCH (c:case)
+ WHERE c.gender='MALE'
+   MATCH (f:file)
+      OPTIONAL MATCH (f)-[*]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+       MATCH (f)-[*]-&gt;(c)
+      OPTIONAL MATCH (f)--&gt;(parent)
+      WITH
+        f, parent, c, a, ct, 
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, a, ct,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, a, ct, unit,
+        round(factor * value)/factor AS size
+      RETURN DISTINCT 
+       f.file_name AS `File Name`,
+       head(labels(parent)) as Association,
+       f.file_description AS Description,
+       f.file_format AS `File Format`,
+         CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+       ct.clinical_trial_designation AS `Trial Code`,
+       a.arm_id AS Arm,
+       c.case_id AS `Case ID`
+        </t>
   </si>
 </sst>
 </file>
@@ -467,19 +486,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -496,15 +515,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -513,15 +532,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
updated CTDC 1 script
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D356F9-3AE1-4CDC-9E10-C8B0D58BBE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9622802E-1F03-4907-93FE-9234377B718E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -486,19 +486,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
added files tab for ctdc and gender female script
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D356F9-3AE1-4CDC-9E10-C8B0D58BBE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D49340D-0D3E-48FF-A33E-FA57BF4A1902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>

</xml_diff>

<commit_message>
ctdc pubmed id and trial arm
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Gender-Male.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D49340D-0D3E-48FF-A33E-FA57BF4A1902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6B4F25-1B9C-4459-BFBE-750CD8D666ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -74,15 +74,6 @@
     c.race AS Race,
     c.ethnicity AS Ethnicity
  </t>
-  </si>
-  <si>
-    <t>MATCH (s:specimen)--&gt;(c:case)--&gt;(:arm)--&gt;(ct:clinical_trial)
-    WHERE c.gender = "MALE"
-OPTIONAL MATCH (f:file)--&gt;(:sequencing_assay)--&gt;(:nucleic_acid)--&gt;(s)
-RETURN 
-     COUNT(DISTINCT ct.clinical_trial_designation) AS Trials,
-     COUNT(DISTINCT c.case_id) AS Cases,
-      COUNT(DISTINCT f) AS Files</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -115,6 +106,15 @@
        a.arm_id AS Arm,
        c.case_id AS `Case ID`
         </t>
+  </si>
+  <si>
+    <t>MATCH (s:specimen)--&gt;(c:case)--&gt;(a:arm)--&gt;(ct:clinical_trial)
+    WHERE c.gender = "MALE"
+OPTIONAL MATCH (f:file)--&gt;(:sequencing_assay)--&gt;(:nucleic_acid)--&gt;(s)
+RETURN 
+     COUNT(DISTINCT ct.clinical_trial_designation) AS Trials,
+     COUNT(DISTINCT c.case_id) AS Cases,
+      COUNT(DISTINCT f) AS Files</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -537,10 +537,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>

</xml_diff>